<commit_message>
Resimulated everything with psize params
</commit_message>
<xml_diff>
--- a/PAA/Hydration_Energies.xlsx
+++ b/PAA/Hydration_Energies.xlsx
@@ -9,22 +9,32 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7692"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7692" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hydration_Energies" sheetId="1" r:id="rId1"/>
+    <sheet name="Hydration_all" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Size</t>
   </si>
   <si>
     <t>HydrationEnergy</t>
+  </si>
+  <si>
+    <t>HydrationEnergy_kJperMol</t>
+  </si>
+  <si>
+    <t>Hyd2</t>
+  </si>
+  <si>
+    <t>psize params run</t>
   </si>
 </sst>
 </file>
@@ -508,8 +518,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -833,7 +844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -914,4 +925,145 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>-29853.523000000001</v>
+      </c>
+      <c r="C2">
+        <v>-25304.7703</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-28413.667369440001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>-32100</v>
+      </c>
+      <c r="C3">
+        <v>-27099.15</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-77711.659220169997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>-43537.3</v>
+      </c>
+      <c r="C4">
+        <v>-32838.676800000001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-75392.540148309999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>-37961.97</v>
+      </c>
+      <c r="C5">
+        <v>-37961.97</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-82534.183866730004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>-39400</v>
+      </c>
+      <c r="C6">
+        <v>-39400</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-83708.873504570001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>-19845.761299999998</v>
+      </c>
+      <c r="C7">
+        <v>-19845.761299999998</v>
+      </c>
+      <c r="D7" s="1">
+        <v>12110.654760789999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <v>-20155.915000000001</v>
+      </c>
+      <c r="C8">
+        <v>-20155.915000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>-33756.466999999997</v>
+      </c>
+      <c r="C9">
+        <v>-33756.466999999997</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-107927.2195149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
renamed (file name) 30 unit ions and obtained PAA 20 unit structures from 30 unit
</commit_message>
<xml_diff>
--- a/PAA/Hydration_Energies.xlsx
+++ b/PAA/Hydration_Energies.xlsx
@@ -932,7 +932,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,7 +1035,7 @@
         <v>-19845.761299999998</v>
       </c>
       <c r="D7" s="1">
-        <v>12110.654760789999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1047,6 +1047,9 @@
       </c>
       <c r="C8">
         <v>-20155.915000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>